<commit_message>
Change calc function to return a series of values instead of just final net worth
</commit_message>
<xml_diff>
--- a/FICalculator.xlsx
+++ b/FICalculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11900"/>
   </bookViews>
   <sheets>
     <sheet name="Compounded Annually" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Monthly</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Monthly with Principle Growth</t>
+  </si>
+  <si>
+    <t>Annually with Principle +  growth, negative net worth</t>
   </si>
 </sst>
 </file>
@@ -395,15 +398,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -413,8 +419,11 @@
       <c r="K1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -454,8 +463,23 @@
       <c r="O2">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>-100000</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>40000</v>
+      </c>
+      <c r="U2">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -499,8 +523,25 @@
       <c r="O3">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <f>R2*S2+T2</f>
+        <v>-60000</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f>T2*U2</f>
+        <v>41200</v>
+      </c>
+      <c r="U3">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -518,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <f>G3*H3+I3</f>
+        <f t="shared" ref="G4:G63" si="0">G3*H3+I3</f>
         <v>-20000</v>
       </c>
       <c r="H4">
@@ -544,8 +585,25 @@
       <c r="O4">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <f>R3*S3+T3</f>
+        <v>-18800</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <f>T3*U3</f>
+        <v>42436</v>
+      </c>
+      <c r="U4">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -563,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <f>G4*H4+I4</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="H5">
@@ -576,21 +634,38 @@
         <v>3</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L64" si="0">L4*M4+N4</f>
+        <f t="shared" ref="L5:L64" si="1">L4*M4+N4</f>
         <v>254820.30000000002</v>
       </c>
       <c r="M5">
         <v>1.07</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N62" si="1">N4*O4</f>
+        <f t="shared" ref="N5:N62" si="2">N4*O4</f>
         <v>43709.08</v>
       </c>
       <c r="O5">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <f>R4*S4+T4</f>
+        <v>23636</v>
+      </c>
+      <c r="S5">
+        <v>1.07</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T39" si="3">T4*U4</f>
+        <v>43709.08</v>
+      </c>
+      <c r="U5">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -608,7 +683,7 @@
         <v>4</v>
       </c>
       <c r="G6">
-        <f>G5*H5+I5</f>
+        <f t="shared" si="0"/>
         <v>61400</v>
       </c>
       <c r="H6">
@@ -621,21 +696,38 @@
         <v>4</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>316366.80100000004</v>
       </c>
       <c r="M6">
         <v>1.07</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45020.352400000003</v>
       </c>
       <c r="O6">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <f>R5*S5+T5</f>
+        <v>68999.600000000006</v>
+      </c>
+      <c r="S6">
+        <v>1.07</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>45020.352400000003</v>
+      </c>
+      <c r="U6">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -653,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <f>G6*H6+I6</f>
+        <f t="shared" si="0"/>
         <v>105698</v>
       </c>
       <c r="H7">
@@ -666,21 +758,38 @@
         <v>5</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>383532.82947000011</v>
       </c>
       <c r="M7">
         <v>1.07</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46370.962972000001</v>
       </c>
       <c r="O7">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <f>R6*S6+T6</f>
+        <v>118849.92440000002</v>
+      </c>
+      <c r="S7">
+        <v>1.07</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>46370.962972000001</v>
+      </c>
+      <c r="U7">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -698,7 +807,7 @@
         <v>6</v>
       </c>
       <c r="G8">
-        <f>G7*H7+I7</f>
+        <f t="shared" si="0"/>
         <v>153096.85999999999</v>
       </c>
       <c r="H8">
@@ -711,21 +820,38 @@
         <v>6</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>456751.09050490014</v>
       </c>
       <c r="M8">
         <v>1.07</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47762.091861159999</v>
       </c>
       <c r="O8">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <f>R7*S7+T7</f>
+        <v>173540.38208000004</v>
+      </c>
+      <c r="S8">
+        <v>1.07</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>47762.091861159999</v>
+      </c>
+      <c r="U8">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -743,7 +869,7 @@
         <v>7</v>
       </c>
       <c r="G9">
-        <f>G8*H8+I8</f>
+        <f t="shared" si="0"/>
         <v>203813.64019999999</v>
       </c>
       <c r="H9">
@@ -756,21 +882,38 @@
         <v>7</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>536485.75870140316</v>
       </c>
       <c r="M9">
         <v>1.07</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49194.954616994801</v>
       </c>
       <c r="O9">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9">
+        <f>R8*S8+T8</f>
+        <v>233450.30068676005</v>
+      </c>
+      <c r="S9">
+        <v>1.07</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>49194.954616994801</v>
+      </c>
+      <c r="U9">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -788,7 +931,7 @@
         <v>8</v>
       </c>
       <c r="G10">
-        <f>G9*H9+I9</f>
+        <f t="shared" si="0"/>
         <v>258080.59501400002</v>
       </c>
       <c r="H10">
@@ -801,21 +944,38 @@
         <v>8</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>623234.71642749629</v>
       </c>
       <c r="M10">
         <v>1.07</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50670.803255504645</v>
       </c>
       <c r="O10">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <f>R9*S9+T9</f>
+        <v>298986.77635182807</v>
+      </c>
+      <c r="S10">
+        <v>1.07</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="3"/>
+        <v>50670.803255504645</v>
+      </c>
+      <c r="U10">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -833,7 +993,7 @@
         <v>9</v>
       </c>
       <c r="G11">
-        <f>G10*H10+I10</f>
+        <f t="shared" si="0"/>
         <v>316146.23666498001</v>
       </c>
       <c r="H11">
@@ -846,21 +1006,38 @@
         <v>9</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>717531.94983292581</v>
       </c>
       <c r="M11">
         <v>1.07</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52190.927353169784</v>
       </c>
       <c r="O11">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q11">
+        <v>9</v>
+      </c>
+      <c r="R11">
+        <f>R10*S10+T10</f>
+        <v>370586.65395196067</v>
+      </c>
+      <c r="S11">
+        <v>1.07</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>52190.927353169784</v>
+      </c>
+      <c r="U11">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -878,7 +1055,7 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <f>G11*H11+I11</f>
+        <f t="shared" si="0"/>
         <v>378276.47323152865</v>
       </c>
       <c r="H12">
@@ -891,21 +1068,38 @@
         <v>10</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>819950.11367440037</v>
       </c>
       <c r="M12">
         <v>1.07</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53756.655173764877</v>
       </c>
       <c r="O12">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12">
+        <f>R11*S11+T11</f>
+        <v>448718.64708176773</v>
+      </c>
+      <c r="S12">
+        <v>1.07</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>53756.655173764877</v>
+      </c>
+      <c r="U12">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -923,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <f>G12*H12+I12</f>
+        <f t="shared" si="0"/>
         <v>444755.82635773567</v>
       </c>
       <c r="H13">
@@ -936,21 +1130,38 @@
         <v>11</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>931103.27680537337</v>
       </c>
       <c r="M13">
         <v>1.07</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55369.354828977826</v>
       </c>
       <c r="O13">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <f>R12*S12+T12</f>
+        <v>533885.60755125643</v>
+      </c>
+      <c r="S13">
+        <v>1.07</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="3"/>
+        <v>55369.354828977826</v>
+      </c>
+      <c r="U13">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -968,7 +1179,7 @@
         <v>12</v>
       </c>
       <c r="G14">
-        <f>G13*H13+I13</f>
+        <f t="shared" si="0"/>
         <v>515888.73420277721</v>
       </c>
       <c r="H14">
@@ -981,21 +1192,38 @@
         <v>12</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1051649.8610107272</v>
       </c>
       <c r="M14">
         <v>1.07</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57030.435473847159</v>
       </c>
       <c r="O14">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="R14">
+        <f>R13*S13+T13</f>
+        <v>626626.9549088222</v>
+      </c>
+      <c r="S14">
+        <v>1.07</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="3"/>
+        <v>57030.435473847159</v>
+      </c>
+      <c r="U14">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1013,7 +1241,7 @@
         <v>13</v>
       </c>
       <c r="G15">
-        <f>G14*H14+I14</f>
+        <f t="shared" si="0"/>
         <v>592000.94559697167</v>
       </c>
       <c r="H15">
@@ -1026,21 +1254,38 @@
         <v>13</v>
       </c>
       <c r="L15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1182295.7867553255</v>
       </c>
       <c r="M15">
         <v>1.07</v>
       </c>
       <c r="N15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58741.348538062579</v>
       </c>
       <c r="O15">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q15">
+        <v>13</v>
+      </c>
+      <c r="R15">
+        <f>R14*S14+T14</f>
+        <v>727521.27722628694</v>
+      </c>
+      <c r="S15">
+        <v>1.07</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
+        <v>58741.348538062579</v>
+      </c>
+      <c r="U15">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1058,7 +1303,7 @@
         <v>14</v>
       </c>
       <c r="G16">
-        <f>G15*H15+I15</f>
+        <f t="shared" si="0"/>
         <v>673441.01178875973</v>
       </c>
       <c r="H16">
@@ -1071,21 +1316,38 @@
         <v>14</v>
       </c>
       <c r="L16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1323797.8403662608</v>
       </c>
       <c r="M16">
         <v>1.07</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60503.58899420446</v>
       </c>
       <c r="O16">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q16">
+        <v>14</v>
+      </c>
+      <c r="R16">
+        <f>R15*S15+T15</f>
+        <v>837189.11517018965</v>
+      </c>
+      <c r="S16">
+        <v>1.07</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="3"/>
+        <v>60503.58899420446</v>
+      </c>
+      <c r="U16">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1103,7 +1365,7 @@
         <v>15</v>
       </c>
       <c r="G17">
-        <f>G16*H16+I16</f>
+        <f t="shared" si="0"/>
         <v>760581.88261397299</v>
       </c>
       <c r="H17">
@@ -1116,21 +1378,38 @@
         <v>15</v>
       </c>
       <c r="L17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1476967.2781861038</v>
       </c>
       <c r="M17">
         <v>1.07</v>
       </c>
       <c r="N17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62318.696664030598</v>
       </c>
       <c r="O17">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q17">
+        <v>15</v>
+      </c>
+      <c r="R17">
+        <f>R16*S16+T16</f>
+        <v>956295.94222630735</v>
+      </c>
+      <c r="S17">
+        <v>1.07</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="3"/>
+        <v>62318.696664030598</v>
+      </c>
+      <c r="U17">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1148,7 +1427,7 @@
         <v>16</v>
       </c>
       <c r="G18">
-        <f>G17*H17+I17</f>
+        <f t="shared" si="0"/>
         <v>853822.61439695116</v>
       </c>
       <c r="H18">
@@ -1161,21 +1440,38 @@
         <v>16</v>
       </c>
       <c r="L18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1642673.6843231618</v>
       </c>
       <c r="M18">
         <v>1.07</v>
       </c>
       <c r="N18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64188.25756395152</v>
       </c>
       <c r="O18">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q18">
+        <v>16</v>
+      </c>
+      <c r="R18">
+        <f>R17*S17+T17</f>
+        <v>1085555.3548461795</v>
+      </c>
+      <c r="S18">
+        <v>1.07</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>64188.25756395152</v>
+      </c>
+      <c r="U18">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1193,7 +1489,7 @@
         <v>17</v>
       </c>
       <c r="G19">
-        <f>G18*H18+I18</f>
+        <f t="shared" si="0"/>
         <v>953590.19740473782</v>
       </c>
       <c r="H19">
@@ -1206,21 +1502,38 @@
         <v>17</v>
       </c>
       <c r="L19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1821849.0997897347</v>
       </c>
       <c r="M19">
         <v>1.07</v>
       </c>
       <c r="N19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66113.905290870069</v>
       </c>
       <c r="O19">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q19">
+        <v>17</v>
+      </c>
+      <c r="R19">
+        <f>R18*S18+T18</f>
+        <v>1225732.4872493634</v>
+      </c>
+      <c r="S19">
+        <v>1.07</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>66113.905290870069</v>
+      </c>
+      <c r="U19">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1238,7 +1551,7 @@
         <v>18</v>
       </c>
       <c r="G20">
-        <f>G19*H19+I19</f>
+        <f t="shared" si="0"/>
         <v>1060341.5112230694</v>
       </c>
       <c r="H20">
@@ -1251,21 +1564,38 @@
         <v>18</v>
       </c>
       <c r="L20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2015492.4420658862</v>
       </c>
       <c r="M20">
         <v>1.07</v>
       </c>
       <c r="N20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68097.322449596177</v>
       </c>
       <c r="O20">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q20">
+        <v>18</v>
+      </c>
+      <c r="R20">
+        <f>R19*S19+T19</f>
+        <v>1377647.666647689</v>
+      </c>
+      <c r="S20">
+        <v>1.07</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>68097.322449596177</v>
+      </c>
+      <c r="U20">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1283,7 +1613,7 @@
         <v>19</v>
       </c>
       <c r="G21">
-        <f>G20*H20+I20</f>
+        <f t="shared" si="0"/>
         <v>1174565.4170086842</v>
       </c>
       <c r="H21">
@@ -1296,21 +1626,38 @@
         <v>19</v>
       </c>
       <c r="L21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2224674.2354600946</v>
       </c>
       <c r="M21">
         <v>1.07</v>
       </c>
       <c r="N21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70140.24212308407</v>
       </c>
       <c r="O21">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q21">
+        <v>19</v>
+      </c>
+      <c r="R21">
+        <f>R20*S20+T20</f>
+        <v>1542180.3257626235</v>
+      </c>
+      <c r="S21">
+        <v>1.07</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>70140.24212308407</v>
+      </c>
+      <c r="U21">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1328,7 +1675,7 @@
         <v>20</v>
       </c>
       <c r="G22">
-        <f>G21*H21+I21</f>
+        <f t="shared" si="0"/>
         <v>1296784.9961992921</v>
       </c>
       <c r="H22">
@@ -1341,21 +1688,38 @@
         <v>20</v>
       </c>
       <c r="L22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2450541.6740653855</v>
       </c>
       <c r="M22">
         <v>1.07</v>
       </c>
       <c r="N22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72244.4493867766</v>
       </c>
       <c r="O22">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q22">
+        <v>20</v>
+      </c>
+      <c r="R22">
+        <f>R21*S21+T21</f>
+        <v>1720273.1906890913</v>
+      </c>
+      <c r="S22">
+        <v>1.07</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>72244.4493867766</v>
+      </c>
+      <c r="U22">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1373,7 +1737,7 @@
         <v>21</v>
       </c>
       <c r="G23">
-        <f>G22*H22+I22</f>
+        <f t="shared" si="0"/>
         <v>1427559.9459332426</v>
       </c>
       <c r="H23">
@@ -1386,21 +1750,38 @@
         <v>21</v>
       </c>
       <c r="L23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2694324.0406367392</v>
       </c>
       <c r="M23">
         <v>1.07</v>
       </c>
       <c r="N23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74411.782868379902</v>
       </c>
       <c r="O23">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q23">
+        <v>21</v>
+      </c>
+      <c r="R23">
+        <f>R22*S22+T22</f>
+        <v>1912936.7634241045</v>
+      </c>
+      <c r="S23">
+        <v>1.07</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="3"/>
+        <v>74411.782868379902</v>
+      </c>
+      <c r="U23">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1418,7 +1799,7 @@
         <v>22</v>
       </c>
       <c r="G24">
-        <f>G23*H23+I23</f>
+        <f t="shared" si="0"/>
         <v>1567489.1421485697</v>
       </c>
       <c r="H24">
@@ -1431,21 +1812,38 @@
         <v>22</v>
       </c>
       <c r="L24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2957338.5063496907</v>
       </c>
       <c r="M24">
         <v>1.07</v>
       </c>
       <c r="N24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76644.136354431306</v>
       </c>
       <c r="O24">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q24">
+        <v>22</v>
+      </c>
+      <c r="R24">
+        <f>R23*S23+T23</f>
+        <v>2121254.1197321718</v>
+      </c>
+      <c r="S24">
+        <v>1.07</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="3"/>
+        <v>76644.136354431306</v>
+      </c>
+      <c r="U24">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1463,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="G25">
-        <f>G24*H24+I24</f>
+        <f t="shared" si="0"/>
         <v>1717213.3820989698</v>
       </c>
       <c r="H25">
@@ -1476,21 +1874,38 @@
         <v>23</v>
       </c>
       <c r="L25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3240996.3381486009</v>
       </c>
       <c r="M25">
         <v>1.07</v>
       </c>
       <c r="N25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78943.460445064251</v>
       </c>
       <c r="O25">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q25">
+        <v>23</v>
+      </c>
+      <c r="R25">
+        <f>R24*S24+T24</f>
+        <v>2346386.0444678552</v>
+      </c>
+      <c r="S25">
+        <v>1.07</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="3"/>
+        <v>78943.460445064251</v>
+      </c>
+      <c r="U25">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1508,7 +1923,7 @@
         <v>24</v>
       </c>
       <c r="G26">
-        <f>G25*H25+I25</f>
+        <f t="shared" si="0"/>
         <v>1877418.3188458977</v>
       </c>
       <c r="H26">
@@ -1521,21 +1936,38 @@
         <v>24</v>
       </c>
       <c r="L26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3546809.5422640671</v>
       </c>
       <c r="M26">
         <v>1.07</v>
       </c>
       <c r="N26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81311.76425841618</v>
       </c>
       <c r="O26">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q26">
+        <v>24</v>
+      </c>
+      <c r="R26">
+        <f>R25*S25+T25</f>
+        <v>2589576.5280256695</v>
+      </c>
+      <c r="S26">
+        <v>1.07</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="3"/>
+        <v>81311.76425841618</v>
+      </c>
+      <c r="U26">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1553,7 +1985,7 @@
         <v>25</v>
       </c>
       <c r="G27">
-        <f>G26*H26+I26</f>
+        <f t="shared" si="0"/>
         <v>2048837.6011651107</v>
       </c>
       <c r="H27">
@@ -1566,21 +1998,38 @@
         <v>25</v>
       </c>
       <c r="L27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3876397.9744809684</v>
       </c>
       <c r="M27">
         <v>1.07</v>
       </c>
       <c r="N27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83751.117186168674</v>
       </c>
       <c r="O27">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q27">
+        <v>25</v>
+      </c>
+      <c r="R27">
+        <f>R26*S26+T26</f>
+        <v>2852158.6492458829</v>
+      </c>
+      <c r="S27">
+        <v>1.07</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="3"/>
+        <v>83751.117186168674</v>
+      </c>
+      <c r="U27">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1598,7 +2047,7 @@
         <v>26</v>
       </c>
       <c r="G28">
-        <f>G27*H27+I27</f>
+        <f t="shared" si="0"/>
         <v>2232256.2332466687</v>
       </c>
       <c r="H28">
@@ -1611,21 +2060,38 @@
         <v>26</v>
       </c>
       <c r="L28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4231496.9498808049</v>
       </c>
       <c r="M28">
         <v>1.07</v>
       </c>
       <c r="N28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86263.650701753737</v>
       </c>
       <c r="O28">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q28">
+        <v>26</v>
+      </c>
+      <c r="R28">
+        <f>R27*S27+T27</f>
+        <v>3135560.8718792633</v>
+      </c>
+      <c r="S28">
+        <v>1.07</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="3"/>
+        <v>86263.650701753737</v>
+      </c>
+      <c r="U28">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1643,7 +2109,7 @@
         <v>27</v>
       </c>
       <c r="G29">
-        <f>G28*H28+I28</f>
+        <f t="shared" si="0"/>
         <v>2428514.1695739357</v>
       </c>
       <c r="H29">
@@ -1656,21 +2122,38 @@
         <v>27</v>
       </c>
       <c r="L29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4613965.3870742153</v>
       </c>
       <c r="M29">
         <v>1.07</v>
       </c>
       <c r="N29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88851.560222806351</v>
       </c>
       <c r="O29">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q29">
+        <v>27</v>
+      </c>
+      <c r="R29">
+        <f>R28*S28+T28</f>
+        <v>3441313.7836125656</v>
+      </c>
+      <c r="S29">
+        <v>1.07</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="3"/>
+        <v>88851.560222806351</v>
+      </c>
+      <c r="U29">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1688,7 +2171,7 @@
         <v>28</v>
       </c>
       <c r="G30">
-        <f>G29*H29+I29</f>
+        <f t="shared" si="0"/>
         <v>2638510.1614441113</v>
       </c>
       <c r="H30">
@@ -1701,21 +2184,38 @@
         <v>28</v>
       </c>
       <c r="L30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5025794.5243922174</v>
       </c>
       <c r="M30">
         <v>1.07</v>
       </c>
       <c r="N30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91517.107029490537</v>
       </c>
       <c r="O30">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q30">
+        <v>28</v>
+      </c>
+      <c r="R30">
+        <f>R29*S29+T29</f>
+        <v>3771057.3086882518</v>
+      </c>
+      <c r="S30">
+        <v>1.07</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>91517.107029490537</v>
+      </c>
+      <c r="U30">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1733,7 +2233,7 @@
         <v>29</v>
       </c>
       <c r="G31">
-        <f>G30*H30+I30</f>
+        <f t="shared" si="0"/>
         <v>2863205.8727451991</v>
       </c>
       <c r="H31">
@@ -1746,21 +2246,38 @@
         <v>29</v>
       </c>
       <c r="L31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5469117.2481291629</v>
       </c>
       <c r="M31">
         <v>1.07</v>
       </c>
       <c r="N31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94262.620240375254</v>
       </c>
       <c r="O31">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q31">
+        <v>29</v>
+      </c>
+      <c r="R31">
+        <f>R30*S30+T30</f>
+        <v>4126548.4273259202</v>
+      </c>
+      <c r="S31">
+        <v>1.07</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="3"/>
+        <v>94262.620240375254</v>
+      </c>
+      <c r="U31">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1778,7 +2295,7 @@
         <v>30</v>
       </c>
       <c r="G32">
-        <f>G31*H31+I31</f>
+        <f t="shared" si="0"/>
         <v>3103630.2838373631</v>
       </c>
       <c r="H32">
@@ -1791,21 +2308,38 @@
         <v>30</v>
       </c>
       <c r="L32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5946218.07573858</v>
       </c>
       <c r="M32">
         <v>1.07</v>
       </c>
       <c r="N32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97090.49884758651</v>
       </c>
       <c r="O32">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q32">
+        <v>30</v>
+      </c>
+      <c r="R32">
+        <f>R31*S31+T31</f>
+        <v>4509669.4374791104</v>
+      </c>
+      <c r="S32">
+        <v>1.07</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="3"/>
+        <v>97090.49884758651</v>
+      </c>
+      <c r="U32">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1823,7 +2357,7 @@
         <v>31</v>
       </c>
       <c r="G33">
-        <f>G32*H32+I32</f>
+        <f t="shared" si="0"/>
         <v>3360884.4037059788</v>
       </c>
       <c r="H33">
@@ -1836,21 +2370,38 @@
         <v>31</v>
       </c>
       <c r="L33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6459543.8398878668</v>
       </c>
       <c r="M33">
         <v>1.07</v>
       </c>
       <c r="N33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100003.21381301411</v>
       </c>
       <c r="O33">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q33">
+        <v>31</v>
+      </c>
+      <c r="R33">
+        <f>R32*S32+T32</f>
+        <v>4922436.7969502341</v>
+      </c>
+      <c r="S33">
+        <v>1.07</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="3"/>
+        <v>100003.21381301411</v>
+      </c>
+      <c r="U33">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1868,7 +2419,7 @@
         <v>32</v>
       </c>
       <c r="G34">
-        <f>G33*H33+I33</f>
+        <f t="shared" si="0"/>
         <v>3636146.3119653976</v>
       </c>
       <c r="H34">
@@ -1881,21 +2432,38 @@
         <v>32</v>
       </c>
       <c r="L34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7011715.1224930324</v>
       </c>
       <c r="M34">
         <v>1.07</v>
       </c>
       <c r="N34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103003.31022740454</v>
       </c>
       <c r="O34">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q34">
+        <v>32</v>
+      </c>
+      <c r="R34">
+        <f>R33*S33+T33</f>
+        <v>5367010.5865497654</v>
+      </c>
+      <c r="S34">
+        <v>1.07</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="3"/>
+        <v>103003.31022740454</v>
+      </c>
+      <c r="U34">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1913,7 +2481,7 @@
         <v>33</v>
       </c>
       <c r="G35">
-        <f>G34*H34+I34</f>
+        <f t="shared" si="0"/>
         <v>3930676.5538029755</v>
       </c>
       <c r="H35">
@@ -1926,21 +2494,38 @@
         <v>33</v>
       </c>
       <c r="L35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7605538.4912949493</v>
       </c>
       <c r="M35">
         <v>1.07</v>
       </c>
       <c r="N35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106093.40953422668</v>
       </c>
       <c r="O35">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q35">
+        <v>33</v>
+      </c>
+      <c r="R35">
+        <f>R34*S34+T34</f>
+        <v>5845704.6378356535</v>
+      </c>
+      <c r="S35">
+        <v>1.07</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="3"/>
+        <v>106093.40953422668</v>
+      </c>
+      <c r="U35">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1958,7 +2543,7 @@
         <v>34</v>
       </c>
       <c r="G36">
-        <f>G35*H35+I35</f>
+        <f t="shared" si="0"/>
         <v>4245823.9125691839</v>
       </c>
       <c r="H36">
@@ -1971,21 +2556,38 @@
         <v>34</v>
       </c>
       <c r="L36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8244019.5952198235</v>
       </c>
       <c r="M36">
         <v>1.07</v>
       </c>
       <c r="N36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109276.21182025349</v>
       </c>
       <c r="O36">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q36">
+        <v>34</v>
+      </c>
+      <c r="R36">
+        <f>R35*S35+T35</f>
+        <v>6360997.3720183764</v>
+      </c>
+      <c r="S36">
+        <v>1.07</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>109276.21182025349</v>
+      </c>
+      <c r="U36">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2003,7 +2605,7 @@
         <v>35</v>
       </c>
       <c r="G37">
-        <f>G36*H36+I36</f>
+        <f t="shared" si="0"/>
         <v>4583031.5864490271</v>
       </c>
       <c r="H37">
@@ -2016,21 +2618,38 @@
         <v>35</v>
       </c>
       <c r="L37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8930377.178705465</v>
       </c>
       <c r="M37">
         <v>1.07</v>
       </c>
       <c r="N37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112554.4981748611</v>
       </c>
       <c r="O37">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q37">
+        <v>35</v>
+      </c>
+      <c r="R37">
+        <f>R36*S36+T36</f>
+        <v>6915543.3998799166</v>
+      </c>
+      <c r="S37">
+        <v>1.07</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="3"/>
+        <v>112554.4981748611</v>
+      </c>
+      <c r="U37">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2048,7 +2667,7 @@
         <v>36</v>
       </c>
       <c r="G38">
-        <f>G37*H37+I37</f>
+        <f t="shared" si="0"/>
         <v>4943843.7975004595</v>
       </c>
       <c r="H38">
@@ -2061,21 +2680,38 @@
         <v>36</v>
       </c>
       <c r="L38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9668058.07938971</v>
       </c>
       <c r="M38">
         <v>1.07</v>
       </c>
       <c r="N38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115931.13312010694</v>
       </c>
       <c r="O38">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q38">
+        <v>36</v>
+      </c>
+      <c r="R38">
+        <f>R37*S37+T37</f>
+        <v>7512185.9360463722</v>
+      </c>
+      <c r="S38">
+        <v>1.07</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="3"/>
+        <v>115931.13312010694</v>
+      </c>
+      <c r="U38">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2093,7 +2729,7 @@
         <v>37</v>
       </c>
       <c r="G39">
-        <f>G38*H38+I38</f>
+        <f t="shared" si="0"/>
         <v>5329912.8633254915</v>
       </c>
       <c r="H39">
@@ -2106,21 +2742,38 @@
         <v>37</v>
       </c>
       <c r="L39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10460753.278067097</v>
       </c>
       <c r="M39">
         <v>1.07</v>
       </c>
       <c r="N39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119409.06711371015</v>
       </c>
       <c r="O39">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q39">
+        <v>37</v>
+      </c>
+      <c r="R39">
+        <f>R38*S38+T38</f>
+        <v>8153970.0846897252</v>
+      </c>
+      <c r="S39">
+        <v>1.07</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="3"/>
+        <v>119409.06711371015</v>
+      </c>
+      <c r="U39">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2138,7 +2791,7 @@
         <v>38</v>
       </c>
       <c r="G40">
-        <f>G39*H39+I39</f>
+        <f t="shared" si="0"/>
         <v>5743006.7637582766</v>
       </c>
       <c r="H40">
@@ -2151,21 +2804,37 @@
         <v>38</v>
       </c>
       <c r="L40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11312415.074645504</v>
       </c>
       <c r="M40">
         <v>1.07</v>
       </c>
       <c r="N40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122991.33912712145</v>
       </c>
       <c r="O40">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q40">
+        <v>38</v>
+      </c>
+      <c r="R40">
+        <f>R39*S39+T39</f>
+        <v>8844157.0577317178</v>
+      </c>
+      <c r="S40">
+        <v>1.07</v>
+      </c>
+      <c r="T40">
+        <v>40000</v>
+      </c>
+      <c r="U40">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2183,7 +2852,7 @@
         <v>39</v>
       </c>
       <c r="G41">
-        <f>G40*H40+I40</f>
+        <f t="shared" si="0"/>
         <v>6185017.2372213565</v>
       </c>
       <c r="H41">
@@ -2196,21 +2865,37 @@
         <v>39</v>
       </c>
       <c r="L41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12227275.468997812</v>
       </c>
       <c r="M41">
         <v>1.07</v>
       </c>
       <c r="N41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126681.07930093509</v>
       </c>
       <c r="O41">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q41">
+        <v>39</v>
+      </c>
+      <c r="R41">
+        <f>R40*S40+T40</f>
+        <v>9503248.051772939</v>
+      </c>
+      <c r="S41">
+        <v>1.07</v>
+      </c>
+      <c r="T41">
+        <v>40000</v>
+      </c>
+      <c r="U41">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2228,7 +2913,7 @@
         <v>40</v>
       </c>
       <c r="G42">
-        <f>G41*H41+I41</f>
+        <f t="shared" si="0"/>
         <v>6657968.4438268514</v>
       </c>
       <c r="H42">
@@ -2241,21 +2926,37 @@
         <v>40</v>
       </c>
       <c r="L42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13209865.831128594</v>
       </c>
       <c r="M42">
         <v>1.07</v>
       </c>
       <c r="N42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130481.51167996315</v>
       </c>
       <c r="O42">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q42">
+        <v>40</v>
+      </c>
+      <c r="R42">
+        <f>R41*S41+T41</f>
+        <v>10208475.415397046</v>
+      </c>
+      <c r="S42">
+        <v>1.07</v>
+      </c>
+      <c r="T42">
+        <v>40000</v>
+      </c>
+      <c r="U42">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2273,7 +2974,7 @@
         <v>41</v>
       </c>
       <c r="G43">
-        <f>G42*H42+I42</f>
+        <f t="shared" si="0"/>
         <v>7164026.2348947311</v>
       </c>
       <c r="H43">
@@ -2286,21 +2987,37 @@
         <v>41</v>
       </c>
       <c r="L43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14265037.950987559</v>
       </c>
       <c r="M43">
         <v>1.07</v>
       </c>
       <c r="N43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134395.95703036204</v>
       </c>
       <c r="O43">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q43">
+        <v>41</v>
+      </c>
+      <c r="R43">
+        <f>R42*S42+T42</f>
+        <v>10963068.694474841</v>
+      </c>
+      <c r="S43">
+        <v>1.07</v>
+      </c>
+      <c r="T43">
+        <v>40000</v>
+      </c>
+      <c r="U43">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2318,7 +3035,7 @@
         <v>42</v>
       </c>
       <c r="G44">
-        <f>G43*H43+I43</f>
+        <f t="shared" si="0"/>
         <v>7705508.0713373628</v>
       </c>
       <c r="H44">
@@ -2331,21 +3048,37 @@
         <v>42</v>
       </c>
       <c r="L44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15397986.564587051</v>
       </c>
       <c r="M44">
         <v>1.07</v>
       </c>
       <c r="N44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>138427.83574127289</v>
       </c>
       <c r="O44">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q44">
+        <v>42</v>
+      </c>
+      <c r="R44">
+        <f>R43*S43+T43</f>
+        <v>11770483.503088079</v>
+      </c>
+      <c r="S44">
+        <v>1.07</v>
+      </c>
+      <c r="T44">
+        <v>40000</v>
+      </c>
+      <c r="U44">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2363,7 +3096,7 @@
         <v>43</v>
       </c>
       <c r="G45">
-        <f>G44*H44+I44</f>
+        <f t="shared" si="0"/>
         <v>8284893.6363309789</v>
       </c>
       <c r="H45">
@@ -2376,21 +3109,37 @@
         <v>43</v>
       </c>
       <c r="L45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16614273.459849417</v>
       </c>
       <c r="M45">
         <v>1.07</v>
       </c>
       <c r="N45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>142580.6708135111</v>
       </c>
       <c r="O45">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q45">
+        <v>43</v>
+      </c>
+      <c r="R45">
+        <f>R44*S44+T44</f>
+        <v>12634417.348304246</v>
+      </c>
+      <c r="S45">
+        <v>1.07</v>
+      </c>
+      <c r="T45">
+        <v>40000</v>
+      </c>
+      <c r="U45">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2408,7 +3157,7 @@
         <v>44</v>
       </c>
       <c r="G46">
-        <f>G45*H45+I45</f>
+        <f t="shared" si="0"/>
         <v>8904836.1908741482</v>
       </c>
       <c r="H46">
@@ -2421,21 +3170,37 @@
         <v>44</v>
       </c>
       <c r="L46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17919853.272852391</v>
       </c>
       <c r="M46">
         <v>1.07</v>
       </c>
       <c r="N46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146858.09093791642</v>
       </c>
       <c r="O46">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q46">
+        <v>44</v>
+      </c>
+      <c r="R46">
+        <f>R45*S45+T45</f>
+        <v>13558826.562685544</v>
+      </c>
+      <c r="S46">
+        <v>1.07</v>
+      </c>
+      <c r="T46">
+        <v>40000</v>
+      </c>
+      <c r="U46">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2453,7 +3218,7 @@
         <v>45</v>
       </c>
       <c r="G47">
-        <f>G46*H46+I46</f>
+        <f t="shared" si="0"/>
         <v>9568174.7242353391</v>
       </c>
       <c r="H47">
@@ -2466,21 +3231,37 @@
         <v>45</v>
       </c>
       <c r="L47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19321101.092889976</v>
       </c>
       <c r="M47">
         <v>1.07</v>
       </c>
       <c r="N47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>151263.83366605392</v>
       </c>
       <c r="O47">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q47">
+        <v>45</v>
+      </c>
+      <c r="R47">
+        <f>R46*S46+T46</f>
+        <v>14547944.422073532</v>
+      </c>
+      <c r="S47">
+        <v>1.07</v>
+      </c>
+      <c r="T47">
+        <v>40000</v>
+      </c>
+      <c r="U47">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2498,7 +3279,7 @@
         <v>46</v>
       </c>
       <c r="G48">
-        <f>G47*H47+I47</f>
+        <f t="shared" si="0"/>
         <v>10277946.954931814</v>
       </c>
       <c r="H48">
@@ -2511,21 +3292,37 @@
         <v>46</v>
       </c>
       <c r="L48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20824842.003058329</v>
       </c>
       <c r="M48">
         <v>1.07</v>
       </c>
       <c r="N48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>155801.74867603555</v>
       </c>
       <c r="O48">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q48">
+        <v>46</v>
+      </c>
+      <c r="R48">
+        <f>R47*S47+T47</f>
+        <v>15606300.531618681</v>
+      </c>
+      <c r="S48">
+        <v>1.07</v>
+      </c>
+      <c r="T48">
+        <v>40000</v>
+      </c>
+      <c r="U48">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2543,7 +3340,7 @@
         <v>47</v>
       </c>
       <c r="G49">
-        <f>G48*H48+I48</f>
+        <f t="shared" si="0"/>
         <v>11037403.241777042</v>
       </c>
       <c r="H49">
@@ -2556,21 +3353,37 @@
         <v>47</v>
       </c>
       <c r="L49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22438382.691948447</v>
       </c>
       <c r="M49">
         <v>1.07</v>
       </c>
       <c r="N49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160475.80113631662</v>
       </c>
       <c r="O49">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q49">
+        <v>47</v>
+      </c>
+      <c r="R49">
+        <f>R48*S48+T48</f>
+        <v>16738741.56883199</v>
+      </c>
+      <c r="S49">
+        <v>1.07</v>
+      </c>
+      <c r="T49">
+        <v>40000</v>
+      </c>
+      <c r="U49">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2588,7 +3401,7 @@
         <v>48</v>
       </c>
       <c r="G50">
-        <f>G49*H49+I49</f>
+        <f t="shared" si="0"/>
         <v>11850021.468701435</v>
       </c>
       <c r="H50">
@@ -2601,21 +3414,37 @@
         <v>48</v>
       </c>
       <c r="L50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24169545.281521156</v>
       </c>
       <c r="M50">
         <v>1.07</v>
       </c>
       <c r="N50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>165290.07517040611</v>
       </c>
       <c r="O50">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q50">
+        <v>48</v>
+      </c>
+      <c r="R50">
+        <f>R49*S49+T49</f>
+        <v>17950453.478650231</v>
+      </c>
+      <c r="S50">
+        <v>1.07</v>
+      </c>
+      <c r="T50">
+        <v>40000</v>
+      </c>
+      <c r="U50">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2633,7 +3462,7 @@
         <v>49</v>
       </c>
       <c r="G51">
-        <f>G50*H50+I50</f>
+        <f t="shared" si="0"/>
         <v>12719522.971510537</v>
       </c>
       <c r="H51">
@@ -2646,21 +3475,37 @@
         <v>49</v>
       </c>
       <c r="L51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26026703.526398044</v>
       </c>
       <c r="M51">
         <v>1.07</v>
       </c>
       <c r="N51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170248.77742551829</v>
       </c>
       <c r="O51">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q51">
+        <v>49</v>
+      </c>
+      <c r="R51">
+        <f>R50*S50+T50</f>
+        <v>19246985.22215575</v>
+      </c>
+      <c r="S51">
+        <v>1.07</v>
+      </c>
+      <c r="T51">
+        <v>40000</v>
+      </c>
+      <c r="U51">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2678,7 +3523,7 @@
         <v>50</v>
       </c>
       <c r="G52">
-        <f>G51*H51+I51</f>
+        <f t="shared" si="0"/>
         <v>13649889.579516275</v>
       </c>
       <c r="H52">
@@ -2691,21 +3536,37 @@
         <v>50</v>
       </c>
       <c r="L52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28018821.550671428</v>
       </c>
       <c r="M52">
         <v>1.07</v>
       </c>
       <c r="N52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>175356.24074828383</v>
       </c>
       <c r="O52">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q52">
+        <v>50</v>
+      </c>
+      <c r="R52">
+        <f>R51*S51+T51</f>
+        <v>20634274.187706653</v>
+      </c>
+      <c r="S52">
+        <v>1.07</v>
+      </c>
+      <c r="T52">
+        <v>40000</v>
+      </c>
+      <c r="U52">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2723,7 +3584,7 @@
         <v>51</v>
       </c>
       <c r="G53">
-        <f>G52*H52+I52</f>
+        <f t="shared" si="0"/>
         <v>14645381.850082414</v>
       </c>
       <c r="H53">
@@ -2736,21 +3597,37 @@
         <v>51</v>
       </c>
       <c r="L53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30155495.299966712</v>
       </c>
       <c r="M53">
         <v>1.07</v>
       </c>
       <c r="N53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180616.92797073236</v>
       </c>
       <c r="O53">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q53">
+        <v>51</v>
+      </c>
+      <c r="R53">
+        <f>R52*S52+T52</f>
+        <v>22118673.38084612</v>
+      </c>
+      <c r="S53">
+        <v>1.07</v>
+      </c>
+      <c r="T53">
+        <v>40000</v>
+      </c>
+      <c r="U53">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2768,7 +3645,7 @@
         <v>52</v>
       </c>
       <c r="G54">
-        <f>G53*H53+I53</f>
+        <f t="shared" si="0"/>
         <v>15710558.579588184</v>
       </c>
       <c r="H54">
@@ -2781,21 +3658,37 @@
         <v>52</v>
       </c>
       <c r="L54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32446996.898935117</v>
       </c>
       <c r="M54">
         <v>1.07</v>
       </c>
       <c r="N54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>186035.43580985433</v>
       </c>
       <c r="O54">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q54">
+        <v>52</v>
+      </c>
+      <c r="R54">
+        <f>R53*S53+T53</f>
+        <v>23706980.517505351</v>
+      </c>
+      <c r="S54">
+        <v>1.07</v>
+      </c>
+      <c r="T54">
+        <v>40000</v>
+      </c>
+      <c r="U54">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2813,7 +3706,7 @@
         <v>53</v>
       </c>
       <c r="G55">
-        <f>G54*H54+I54</f>
+        <f t="shared" si="0"/>
         <v>16850297.680159356</v>
       </c>
       <c r="H55">
@@ -2826,21 +3719,37 @@
         <v>53</v>
       </c>
       <c r="L55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34904322.117670424</v>
       </c>
       <c r="M55">
         <v>1.07</v>
       </c>
       <c r="N55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>191616.49888414997</v>
       </c>
       <c r="O55">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q55">
+        <v>53</v>
+      </c>
+      <c r="R55">
+        <f>R54*S54+T54</f>
+        <v>25406469.153730728</v>
+      </c>
+      <c r="S55">
+        <v>1.07</v>
+      </c>
+      <c r="T55">
+        <v>40000</v>
+      </c>
+      <c r="U55">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2858,7 +3767,7 @@
         <v>54</v>
       </c>
       <c r="G56">
-        <f>G55*H55+I55</f>
+        <f t="shared" si="0"/>
         <v>18069818.517770514</v>
       </c>
       <c r="H56">
@@ -2871,21 +3780,37 @@
         <v>54</v>
       </c>
       <c r="L56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37539241.164791502</v>
       </c>
       <c r="M56">
         <v>1.07</v>
       </c>
       <c r="N56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>197364.99385067448</v>
       </c>
       <c r="O56">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q56">
+        <v>54</v>
+      </c>
+      <c r="R56">
+        <f>R55*S55+T55</f>
+        <v>27224921.994491879</v>
+      </c>
+      <c r="S56">
+        <v>1.07</v>
+      </c>
+      <c r="T56">
+        <v>40000</v>
+      </c>
+      <c r="U56">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2903,7 +3828,7 @@
         <v>55</v>
       </c>
       <c r="G57">
-        <f>G56*H56+I56</f>
+        <f t="shared" si="0"/>
         <v>19374705.81401445</v>
       </c>
       <c r="H57">
@@ -2916,21 +3841,37 @@
         <v>55</v>
       </c>
       <c r="L57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40364353.040177584</v>
       </c>
       <c r="M57">
         <v>1.07</v>
       </c>
       <c r="N57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>203285.94366619471</v>
       </c>
       <c r="O57">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q57">
+        <v>55</v>
+      </c>
+      <c r="R57">
+        <f>R56*S56+T56</f>
+        <v>29170666.53410631</v>
+      </c>
+      <c r="S57">
+        <v>1.07</v>
+      </c>
+      <c r="T57">
+        <v>40000</v>
+      </c>
+      <c r="U57">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2948,7 +3889,7 @@
         <v>56</v>
       </c>
       <c r="G58">
-        <f>G57*H57+I57</f>
+        <f t="shared" si="0"/>
         <v>20770935.220995463</v>
       </c>
       <c r="H58">
@@ -2961,21 +3902,37 @@
         <v>56</v>
       </c>
       <c r="L58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43393143.696656212</v>
       </c>
       <c r="M58">
         <v>1.07</v>
       </c>
       <c r="N58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>209384.52197618055</v>
       </c>
       <c r="O58">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q58">
+        <v>56</v>
+      </c>
+      <c r="R58">
+        <f>R57*S57+T57</f>
+        <v>31252613.191493753</v>
+      </c>
+      <c r="S58">
+        <v>1.07</v>
+      </c>
+      <c r="T58">
+        <v>40000</v>
+      </c>
+      <c r="U58">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2993,7 +3950,7 @@
         <v>57</v>
       </c>
       <c r="G59">
-        <f>G58*H58+I58</f>
+        <f t="shared" si="0"/>
         <v>22264900.686465148</v>
       </c>
       <c r="H59">
@@ -3006,21 +3963,37 @@
         <v>57</v>
       </c>
       <c r="L59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46640048.277398333</v>
       </c>
       <c r="M59">
         <v>1.07</v>
       </c>
       <c r="N59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>215666.05763546596</v>
       </c>
       <c r="O59">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q59">
+        <v>57</v>
+      </c>
+      <c r="R59">
+        <f>R58*S58+T58</f>
+        <v>33480296.114898317</v>
+      </c>
+      <c r="S59">
+        <v>1.07</v>
+      </c>
+      <c r="T59">
+        <v>40000</v>
+      </c>
+      <c r="U59">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3038,7 +4011,7 @@
         <v>58</v>
       </c>
       <c r="G60">
-        <f>G59*H59+I59</f>
+        <f t="shared" si="0"/>
         <v>23863443.734517708</v>
       </c>
       <c r="H60">
@@ -3051,21 +4024,37 @@
         <v>58</v>
       </c>
       <c r="L60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50120517.714451686</v>
       </c>
       <c r="M60">
         <v>1.07</v>
       </c>
       <c r="N60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>222136.03936452995</v>
       </c>
       <c r="O60">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q60">
+        <v>58</v>
+      </c>
+      <c r="R60">
+        <f>R59*S59+T59</f>
+        <v>35863916.842941202</v>
+      </c>
+      <c r="S60">
+        <v>1.07</v>
+      </c>
+      <c r="T60">
+        <v>40000</v>
+      </c>
+      <c r="U60">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B61">
         <f>B60*C60+D60</f>
         <v>35790147.679880947</v>
@@ -3077,7 +4066,7 @@
         <v>40000</v>
       </c>
       <c r="G61">
-        <f>G60*H60+I60</f>
+        <f t="shared" si="0"/>
         <v>25573884.795933951</v>
       </c>
       <c r="H61">
@@ -3090,21 +4079,34 @@
         <v>59</v>
       </c>
       <c r="L61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53851089.993827835</v>
       </c>
       <c r="M61">
         <v>1.07</v>
       </c>
       <c r="N61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>228800.12054546585</v>
       </c>
       <c r="O61">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R61">
+        <f>R60*S60+T60</f>
+        <v>38414391.021947086</v>
+      </c>
+      <c r="S61">
+        <v>1.07</v>
+      </c>
+      <c r="T61">
+        <v>40000</v>
+      </c>
+      <c r="U61">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B62">
         <f>B61*C61+D61</f>
         <v>38335458.017472617</v>
@@ -3116,7 +4118,7 @@
         <v>40000</v>
       </c>
       <c r="G62">
-        <f>G61*H61+I61</f>
+        <f t="shared" si="0"/>
         <v>27404056.731649328</v>
       </c>
       <c r="H62">
@@ -3129,47 +4131,67 @@
         <v>60</v>
       </c>
       <c r="L62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57849466.413941257</v>
       </c>
       <c r="M62">
         <v>1.07</v>
       </c>
       <c r="N62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>235664.12416182982</v>
       </c>
       <c r="O62">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R62">
+        <f>R61*S61+T61</f>
+        <v>41143398.393483385</v>
+      </c>
+      <c r="S62">
+        <v>1.07</v>
+      </c>
+      <c r="T62">
+        <v>40000</v>
+      </c>
+      <c r="U62">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B63">
         <f>B62*C62+D62</f>
         <v>41058940.0786957</v>
       </c>
       <c r="G63">
-        <f>G62*H62+I62</f>
+        <f t="shared" si="0"/>
         <v>29362340.702864781</v>
       </c>
       <c r="K63">
         <v>61</v>
       </c>
       <c r="L63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62134593.187078983</v>
       </c>
       <c r="O63">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="R63">
+        <f>R62*S62+T62</f>
+        <v>44063436.281027228</v>
+      </c>
+      <c r="U63">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B64">
         <f>B63*C63+D63</f>
         <v>0</v>
       </c>
       <c r="L64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3183,8 +4205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update excel calculation validator
</commit_message>
<xml_diff>
--- a/FICalculator.xlsx
+++ b/FICalculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compounded Annually" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Monthly</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Annually with Principle +  growth, negative net worth</t>
+  </si>
+  <si>
+    <t>Monthly with Principle Growth, negative net worth</t>
   </si>
 </sst>
 </file>
@@ -400,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4203,10 +4206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="R63" sqref="R63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4217,9 +4220,11 @@
     <col min="6" max="6" width="15.6328125" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.6328125" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4229,8 +4234,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4273,8 +4281,26 @@
       <c r="O2">
         <v>40000</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>-100000</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>1.03</v>
+      </c>
+      <c r="V2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4320,8 +4346,27 @@
       <c r="O3">
         <v>40000</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <f>R2*S2+T2</f>
+        <v>-100000</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>1.03</v>
+      </c>
+      <c r="V3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4367,8 +4412,27 @@
       <c r="O4">
         <v>40000</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1">
+        <f>R3*S3+T3</f>
+        <v>-100000</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1.03</v>
+      </c>
+      <c r="V4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4414,8 +4478,27 @@
       <c r="O5">
         <v>40000</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="1">
+        <f>R4*S4+T4</f>
+        <v>-100000</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>1.03</v>
+      </c>
+      <c r="V5">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4461,8 +4544,27 @@
       <c r="O6">
         <v>40000</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6" s="1">
+        <f>R5*S5+T5</f>
+        <v>-100000</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1.03</v>
+      </c>
+      <c r="V6">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4508,8 +4610,27 @@
       <c r="O7">
         <v>40000</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" s="1">
+        <f>R6*S6+T6</f>
+        <v>-100000</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>1.03</v>
+      </c>
+      <c r="V7">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4555,8 +4676,27 @@
       <c r="O8">
         <v>40000</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8" s="1">
+        <f>R7*S7+T7</f>
+        <v>-100000</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>1.03</v>
+      </c>
+      <c r="V8">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4602,8 +4742,27 @@
       <c r="O9">
         <v>40000</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9" s="1">
+        <f>R8*S8+T8</f>
+        <v>-100000</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>1.03</v>
+      </c>
+      <c r="V9">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4649,8 +4808,27 @@
       <c r="O10">
         <v>40000</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10" s="1">
+        <f>R9*S9+T9</f>
+        <v>-100000</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>1.03</v>
+      </c>
+      <c r="V10">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4696,8 +4874,27 @@
       <c r="O11">
         <v>40000</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q11">
+        <v>9</v>
+      </c>
+      <c r="R11" s="1">
+        <f>R10*S10+T10</f>
+        <v>-100000</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>1.03</v>
+      </c>
+      <c r="V11">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4743,8 +4940,27 @@
       <c r="O12">
         <v>40000</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12" s="1">
+        <f>R11*S11+T11</f>
+        <v>-100000</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>1.03</v>
+      </c>
+      <c r="V12">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4790,8 +5006,27 @@
       <c r="O13">
         <v>40000</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13" s="1">
+        <f>R12*S12+T12</f>
+        <v>-100000</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>40000</v>
+      </c>
+      <c r="U13">
+        <v>1.03</v>
+      </c>
+      <c r="V13">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4837,8 +5072,27 @@
       <c r="O14">
         <v>40000</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="R14" s="1">
+        <f>R13*S13+T13</f>
+        <v>-60000</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>1.03</v>
+      </c>
+      <c r="V14">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4884,8 +5138,27 @@
       <c r="O15">
         <v>40000</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q15">
+        <v>13</v>
+      </c>
+      <c r="R15" s="1">
+        <f>R14*S14+T14</f>
+        <v>-60000</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>1.03</v>
+      </c>
+      <c r="V15">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4931,8 +5204,27 @@
       <c r="O16">
         <v>40000</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q16">
+        <v>14</v>
+      </c>
+      <c r="R16" s="1">
+        <f>R15*S15+T15</f>
+        <v>-60000</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>1.03</v>
+      </c>
+      <c r="V16">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4978,8 +5270,27 @@
       <c r="O17">
         <v>40000</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q17">
+        <v>15</v>
+      </c>
+      <c r="R17" s="1">
+        <f>R16*S16+T16</f>
+        <v>-60000</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>1.03</v>
+      </c>
+      <c r="V17">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5025,8 +5336,27 @@
       <c r="O18">
         <v>40000</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q18">
+        <v>16</v>
+      </c>
+      <c r="R18" s="1">
+        <f>R17*S17+T17</f>
+        <v>-60000</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>1.03</v>
+      </c>
+      <c r="V18">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5072,8 +5402,27 @@
       <c r="O19">
         <v>40000</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q19">
+        <v>17</v>
+      </c>
+      <c r="R19" s="1">
+        <f>R18*S18+T18</f>
+        <v>-60000</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>1.03</v>
+      </c>
+      <c r="V19">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5119,8 +5468,27 @@
       <c r="O20">
         <v>40000</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q20">
+        <v>18</v>
+      </c>
+      <c r="R20" s="1">
+        <f>R19*S19+T19</f>
+        <v>-60000</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>1.03</v>
+      </c>
+      <c r="V20">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5166,8 +5534,27 @@
       <c r="O21">
         <v>40000</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q21">
+        <v>19</v>
+      </c>
+      <c r="R21" s="1">
+        <f>R20*S20+T20</f>
+        <v>-60000</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>1.03</v>
+      </c>
+      <c r="V21">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5213,8 +5600,27 @@
       <c r="O22">
         <v>40000</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q22">
+        <v>20</v>
+      </c>
+      <c r="R22" s="1">
+        <f>R21*S21+T21</f>
+        <v>-60000</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>1.03</v>
+      </c>
+      <c r="V22">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5260,8 +5666,27 @@
       <c r="O23">
         <v>40000</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q23">
+        <v>21</v>
+      </c>
+      <c r="R23" s="1">
+        <f>R22*S22+T22</f>
+        <v>-60000</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>1.03</v>
+      </c>
+      <c r="V23">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5307,8 +5732,27 @@
       <c r="O24">
         <v>40000</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q24">
+        <v>22</v>
+      </c>
+      <c r="R24" s="1">
+        <f>R23*S23+T23</f>
+        <v>-60000</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>1.03</v>
+      </c>
+      <c r="V24">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5355,8 +5799,28 @@
       <c r="O25">
         <v>40000</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q25">
+        <v>23</v>
+      </c>
+      <c r="R25" s="1">
+        <f>R24*S24+T24</f>
+        <v>-60000</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <f>U24*V24</f>
+        <v>41200</v>
+      </c>
+      <c r="U25">
+        <v>1.03</v>
+      </c>
+      <c r="V25">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5402,8 +5866,27 @@
       <c r="O26">
         <v>41200</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q26">
+        <v>24</v>
+      </c>
+      <c r="R26" s="1">
+        <f>R25*S25+T25</f>
+        <v>-18800</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>1.03</v>
+      </c>
+      <c r="V26">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5449,8 +5932,27 @@
       <c r="O27">
         <v>41200</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q27">
+        <v>25</v>
+      </c>
+      <c r="R27" s="1">
+        <f>R26*S26+T26</f>
+        <v>-18800</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>1.03</v>
+      </c>
+      <c r="V27">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5496,8 +5998,27 @@
       <c r="O28">
         <v>41200</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q28">
+        <v>26</v>
+      </c>
+      <c r="R28" s="1">
+        <f>R27*S27+T27</f>
+        <v>-18800</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>1.03</v>
+      </c>
+      <c r="V28">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5543,8 +6064,27 @@
       <c r="O29">
         <v>41200</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q29">
+        <v>27</v>
+      </c>
+      <c r="R29" s="1">
+        <f>R28*S28+T28</f>
+        <v>-18800</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>1.03</v>
+      </c>
+      <c r="V29">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5590,8 +6130,27 @@
       <c r="O30">
         <v>41200</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q30">
+        <v>28</v>
+      </c>
+      <c r="R30" s="1">
+        <f>R29*S29+T29</f>
+        <v>-18800</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>1.03</v>
+      </c>
+      <c r="V30">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5637,8 +6196,27 @@
       <c r="O31">
         <v>41200</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q31">
+        <v>29</v>
+      </c>
+      <c r="R31" s="1">
+        <f>R30*S30+T30</f>
+        <v>-18800</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>1.03</v>
+      </c>
+      <c r="V31">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5684,8 +6262,27 @@
       <c r="O32">
         <v>41200</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q32">
+        <v>30</v>
+      </c>
+      <c r="R32" s="1">
+        <f>R31*S31+T31</f>
+        <v>-18800</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>1.03</v>
+      </c>
+      <c r="V32">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5731,8 +6328,27 @@
       <c r="O33">
         <v>41200</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q33">
+        <v>31</v>
+      </c>
+      <c r="R33" s="1">
+        <f>R32*S32+T32</f>
+        <v>-18800</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>1.03</v>
+      </c>
+      <c r="V33">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5778,8 +6394,27 @@
       <c r="O34">
         <v>41200</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q34">
+        <v>32</v>
+      </c>
+      <c r="R34" s="1">
+        <f>R33*S33+T33</f>
+        <v>-18800</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>1.03</v>
+      </c>
+      <c r="V34">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5825,8 +6460,27 @@
       <c r="O35">
         <v>41200</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q35">
+        <v>33</v>
+      </c>
+      <c r="R35" s="1">
+        <f>R34*S34+T34</f>
+        <v>-18800</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>1.03</v>
+      </c>
+      <c r="V35">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5872,8 +6526,27 @@
       <c r="O36">
         <v>41200</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q36">
+        <v>34</v>
+      </c>
+      <c r="R36" s="1">
+        <f>R35*S35+T35</f>
+        <v>-18800</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>1.03</v>
+      </c>
+      <c r="V36">
+        <v>41200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5920,8 +6593,28 @@
       <c r="O37">
         <v>42436</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q37">
+        <v>35</v>
+      </c>
+      <c r="R37" s="1">
+        <f>R36*S36+T36</f>
+        <v>-18800</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <f>U36*V36</f>
+        <v>42436</v>
+      </c>
+      <c r="U37">
+        <v>1.03</v>
+      </c>
+      <c r="V37">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5967,8 +6660,28 @@
       <c r="O38">
         <v>42436</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q38">
+        <v>36</v>
+      </c>
+      <c r="R38" s="1">
+        <f>R37*S37+T37</f>
+        <v>23636</v>
+      </c>
+      <c r="S38">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>1.03</v>
+      </c>
+      <c r="V38">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6004,8 +6717,25 @@
       <c r="O39">
         <v>42436</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q39">
+        <v>37</v>
+      </c>
+      <c r="R39" s="1">
+        <f>R38*S38+T38</f>
+        <v>23773.876666666667</v>
+      </c>
+      <c r="S39">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U39">
+        <v>1.03</v>
+      </c>
+      <c r="V39">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6037,8 +6767,25 @@
       <c r="O40">
         <v>42436</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q40">
+        <v>38</v>
+      </c>
+      <c r="R40" s="1">
+        <f t="shared" ref="R40:R50" si="1">R39*S39+T39</f>
+        <v>23912.55761388889</v>
+      </c>
+      <c r="S40">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U40">
+        <v>1.03</v>
+      </c>
+      <c r="V40">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6070,8 +6817,25 @@
       <c r="O41">
         <v>42436</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q41">
+        <v>39</v>
+      </c>
+      <c r="R41" s="1">
+        <f t="shared" si="1"/>
+        <v>24052.047533303241</v>
+      </c>
+      <c r="S41">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U41">
+        <v>1.03</v>
+      </c>
+      <c r="V41">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6103,8 +6867,25 @@
       <c r="O42">
         <v>42436</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q42">
+        <v>40</v>
+      </c>
+      <c r="R42" s="1">
+        <f t="shared" si="1"/>
+        <v>24192.351143914177</v>
+      </c>
+      <c r="S42">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U42">
+        <v>1.03</v>
+      </c>
+      <c r="V42">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6136,8 +6917,25 @@
       <c r="O43">
         <v>42436</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q43">
+        <v>41</v>
+      </c>
+      <c r="R43" s="1">
+        <f t="shared" si="1"/>
+        <v>24333.473192253678</v>
+      </c>
+      <c r="S43">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U43">
+        <v>1.03</v>
+      </c>
+      <c r="V43">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6169,8 +6967,25 @@
       <c r="O44">
         <v>42436</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q44">
+        <v>42</v>
+      </c>
+      <c r="R44" s="1">
+        <f t="shared" si="1"/>
+        <v>24475.418452541824</v>
+      </c>
+      <c r="S44">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U44">
+        <v>1.03</v>
+      </c>
+      <c r="V44">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6202,8 +7017,25 @@
       <c r="O45">
         <v>42436</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q45">
+        <v>43</v>
+      </c>
+      <c r="R45" s="1">
+        <f t="shared" si="1"/>
+        <v>24618.191726848319</v>
+      </c>
+      <c r="S45">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U45">
+        <v>1.03</v>
+      </c>
+      <c r="V45">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6235,8 +7067,25 @@
       <c r="O46">
         <v>42436</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q46">
+        <v>44</v>
+      </c>
+      <c r="R46" s="1">
+        <f t="shared" si="1"/>
+        <v>24761.797845254936</v>
+      </c>
+      <c r="S46">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U46">
+        <v>1.03</v>
+      </c>
+      <c r="V46">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6261,8 +7110,25 @@
       <c r="O47">
         <v>42436</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q47">
+        <v>45</v>
+      </c>
+      <c r="R47" s="1">
+        <f t="shared" si="1"/>
+        <v>24906.241666018923</v>
+      </c>
+      <c r="S47">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U47">
+        <v>1.03</v>
+      </c>
+      <c r="V47">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6287,8 +7153,25 @@
       <c r="O48">
         <v>42436</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q48">
+        <v>46</v>
+      </c>
+      <c r="R48" s="1">
+        <f t="shared" si="1"/>
+        <v>25051.528075737366</v>
+      </c>
+      <c r="S48">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U48">
+        <v>1.03</v>
+      </c>
+      <c r="V48">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6309,8 +7192,29 @@
       <c r="O49">
         <v>42436</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q49">
+        <v>47</v>
+      </c>
+      <c r="R49" s="1">
+        <f t="shared" si="1"/>
+        <v>25197.6619895125</v>
+      </c>
+      <c r="S49">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="T49">
+        <f>U49*V49</f>
+        <v>43709.08</v>
+      </c>
+      <c r="U49">
+        <v>1.03</v>
+      </c>
+      <c r="V49">
+        <v>42436</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6332,78 +7236,303 @@
       <c r="N50">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q50">
+        <v>48</v>
+      </c>
+      <c r="R50" s="1">
+        <f>R49*S49+T49</f>
+        <v>69053.728351117985</v>
+      </c>
+      <c r="S50">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U50">
+        <v>1.03</v>
+      </c>
+      <c r="V50">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="N51">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q51">
+        <v>49</v>
+      </c>
+      <c r="R51" s="1">
+        <f>R50*S50+T50</f>
+        <v>69456.541766499504</v>
+      </c>
+      <c r="S51">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U51">
+        <v>1.03</v>
+      </c>
+      <c r="V51">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="N52">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q52">
+        <v>50</v>
+      </c>
+      <c r="R52" s="1">
+        <f>R51*S51+T51</f>
+        <v>69861.704926804086</v>
+      </c>
+      <c r="S52">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U52">
+        <v>1.03</v>
+      </c>
+      <c r="V52">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="N53">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q53">
+        <v>51</v>
+      </c>
+      <c r="R53" s="1">
+        <f t="shared" ref="R53:R62" si="2">R52*S52+T52</f>
+        <v>70269.231538877109</v>
+      </c>
+      <c r="S53">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U53">
+        <v>1.03</v>
+      </c>
+      <c r="V53">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N54">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q54">
+        <v>52</v>
+      </c>
+      <c r="R54" s="1">
+        <f t="shared" si="2"/>
+        <v>70679.135389520554</v>
+      </c>
+      <c r="S54">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U54">
+        <v>1.03</v>
+      </c>
+      <c r="V54">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N55">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q55">
+        <v>53</v>
+      </c>
+      <c r="R55" s="1">
+        <f t="shared" si="2"/>
+        <v>71091.430345959423</v>
+      </c>
+      <c r="S55">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U55">
+        <v>1.03</v>
+      </c>
+      <c r="V55">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N56">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q56">
+        <v>54</v>
+      </c>
+      <c r="R56" s="1">
+        <f t="shared" si="2"/>
+        <v>71506.130356310852</v>
+      </c>
+      <c r="S56">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U56">
+        <v>1.03</v>
+      </c>
+      <c r="V56">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N57">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q57">
+        <v>55</v>
+      </c>
+      <c r="R57" s="1">
+        <f t="shared" si="2"/>
+        <v>71923.249450055999</v>
+      </c>
+      <c r="S57">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U57">
+        <v>1.03</v>
+      </c>
+      <c r="V57">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N58">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q58">
+        <v>56</v>
+      </c>
+      <c r="R58" s="1">
+        <f t="shared" si="2"/>
+        <v>72342.801738514667</v>
+      </c>
+      <c r="S58">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U58">
+        <v>1.03</v>
+      </c>
+      <c r="V58">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N59">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q59">
+        <v>57</v>
+      </c>
+      <c r="R59" s="1">
+        <f t="shared" si="2"/>
+        <v>72764.801415322669</v>
+      </c>
+      <c r="S59">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U59">
+        <v>1.03</v>
+      </c>
+      <c r="V59">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N60">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q60">
+        <v>58</v>
+      </c>
+      <c r="R60" s="1">
+        <f t="shared" si="2"/>
+        <v>73189.262756912052</v>
+      </c>
+      <c r="S60">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U60">
+        <v>1.03</v>
+      </c>
+      <c r="V60">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N61">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q61">
+        <v>59</v>
+      </c>
+      <c r="R61" s="1">
+        <f t="shared" si="2"/>
+        <v>73616.200122994036</v>
+      </c>
+      <c r="S61">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="T61">
+        <f>U61*V61</f>
+        <v>45020.352400000003</v>
+      </c>
+      <c r="U61">
+        <v>1.03</v>
+      </c>
+      <c r="V61">
+        <v>43709.08</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N62">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="Q62">
+        <v>60</v>
+      </c>
+      <c r="R62" s="1">
+        <f>R61*S61+T61</f>
+        <v>119065.98035704484</v>
+      </c>
+      <c r="S62">
+        <f>7/12/100+1</f>
+        <v>1.0058333333333334</v>
+      </c>
+      <c r="U62">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="N63">
+        <v>1.03</v>
+      </c>
+      <c r="U63">
         <v>1.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the FI calc spreadsheet
</commit_message>
<xml_diff>
--- a/FICalculator.xlsx
+++ b/FICalculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annually" sheetId="1" r:id="rId1"/>
@@ -9474,8 +9474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO44" workbookViewId="0">
-      <selection activeCell="BF51" sqref="BF51:BF61"/>
+    <sheetView tabSelected="1" topLeftCell="AO19" workbookViewId="0">
+      <selection activeCell="BD14" sqref="BD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11414,7 +11414,7 @@
         <v>40000</v>
       </c>
       <c r="BD13">
-        <v>18000</v>
+        <v>60000</v>
       </c>
       <c r="BE13">
         <v>1.02</v>
@@ -11560,7 +11560,7 @@
       </c>
       <c r="AY14" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ14">
         <v>1</v>
@@ -11718,7 +11718,7 @@
       </c>
       <c r="AY15" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ15">
         <v>1</v>
@@ -11876,7 +11876,7 @@
       </c>
       <c r="AY16" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ16">
         <v>1</v>
@@ -12034,7 +12034,7 @@
       </c>
       <c r="AY17" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ17">
         <v>1</v>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="AY18" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ18">
         <v>1</v>
@@ -12350,7 +12350,7 @@
       </c>
       <c r="AY19" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ19">
         <v>1</v>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="AY20" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ20">
         <v>1</v>
@@ -12666,7 +12666,7 @@
       </c>
       <c r="AY21" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ21">
         <v>1</v>
@@ -12824,7 +12824,7 @@
       </c>
       <c r="AY22" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ22">
         <v>1</v>
@@ -12982,7 +12982,7 @@
       </c>
       <c r="AY23" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ23">
         <v>1</v>
@@ -13140,7 +13140,7 @@
       </c>
       <c r="AY24" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ24">
         <v>1</v>
@@ -13313,7 +13313,7 @@
       </c>
       <c r="AY25" s="1">
         <f t="shared" si="13"/>
-        <v>-78000</v>
+        <v>-120000</v>
       </c>
       <c r="AZ25">
         <v>1</v>
@@ -13474,7 +13474,7 @@
       </c>
       <c r="AY26" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ26">
         <v>1</v>
@@ -13630,7 +13630,7 @@
       </c>
       <c r="AY27" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ27">
         <v>1</v>
@@ -13786,7 +13786,7 @@
       </c>
       <c r="AY28" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ28">
         <v>1</v>
@@ -13942,7 +13942,7 @@
       </c>
       <c r="AY29" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ29">
         <v>1</v>
@@ -14098,7 +14098,7 @@
       </c>
       <c r="AY30" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ30">
         <v>1</v>
@@ -14254,7 +14254,7 @@
       </c>
       <c r="AY31" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ31">
         <v>1</v>
@@ -14410,7 +14410,7 @@
       </c>
       <c r="AY32" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ32">
         <v>1</v>
@@ -14566,7 +14566,7 @@
       </c>
       <c r="AY33" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ33">
         <v>1</v>
@@ -14722,7 +14722,7 @@
       </c>
       <c r="AY34" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ34">
         <v>1</v>
@@ -14878,7 +14878,7 @@
       </c>
       <c r="AY35" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ35">
         <v>1</v>
@@ -15034,7 +15034,7 @@
       </c>
       <c r="AY36" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ36">
         <v>1</v>
@@ -15205,7 +15205,7 @@
       </c>
       <c r="AY37" s="1">
         <f t="shared" si="13"/>
-        <v>-98000</v>
+        <v>-140000</v>
       </c>
       <c r="AZ37">
         <v>1</v>
@@ -15367,7 +15367,7 @@
       </c>
       <c r="AY38" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ38">
         <v>1</v>
@@ -15502,7 +15502,7 @@
       </c>
       <c r="AY39" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ39">
         <v>1</v>
@@ -15630,7 +15630,7 @@
       </c>
       <c r="AY40" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ40">
         <v>1</v>
@@ -15758,7 +15758,7 @@
       </c>
       <c r="AY41" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ41">
         <v>1</v>
@@ -15882,7 +15882,7 @@
       </c>
       <c r="AY42" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ42">
         <v>1</v>
@@ -16006,7 +16006,7 @@
       </c>
       <c r="AY43" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ43">
         <v>1</v>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="AY44" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ44">
         <v>1</v>
@@ -16254,7 +16254,7 @@
       </c>
       <c r="AY45" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ45">
         <v>1</v>
@@ -16378,7 +16378,7 @@
       </c>
       <c r="AY46" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ46">
         <v>1</v>
@@ -16488,7 +16488,7 @@
       </c>
       <c r="AY47" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ47">
         <v>1</v>
@@ -16598,7 +16598,7 @@
       </c>
       <c r="AY48" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ48">
         <v>1</v>
@@ -16716,7 +16716,7 @@
       </c>
       <c r="AY49" s="1">
         <f t="shared" si="13"/>
-        <v>-117988</v>
+        <v>-159988</v>
       </c>
       <c r="AZ49">
         <v>1</v>
@@ -16836,7 +16836,7 @@
       </c>
       <c r="AY50" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ50">
         <v>1</v>
@@ -16905,7 +16905,7 @@
       </c>
       <c r="AY51" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ51">
         <v>1</v>
@@ -16974,7 +16974,7 @@
       </c>
       <c r="AY52" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ52">
         <v>1</v>
@@ -17043,7 +17043,7 @@
       </c>
       <c r="AY53" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ53">
         <v>1</v>
@@ -17109,7 +17109,7 @@
       </c>
       <c r="AY54" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ54">
         <v>1</v>
@@ -17175,7 +17175,7 @@
       </c>
       <c r="AY55" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ55">
         <v>1</v>
@@ -17241,7 +17241,7 @@
       </c>
       <c r="AY56" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ56">
         <v>1</v>
@@ -17307,7 +17307,7 @@
       </c>
       <c r="AY57" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ57">
         <v>1</v>
@@ -17373,7 +17373,7 @@
       </c>
       <c r="AY58" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ58">
         <v>1</v>
@@ -17439,7 +17439,7 @@
       </c>
       <c r="AY59" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ59">
         <v>1</v>
@@ -17505,7 +17505,7 @@
       </c>
       <c r="AY60" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ60">
         <v>1</v>
@@ -17583,7 +17583,7 @@
       </c>
       <c r="AY61" s="1">
         <f t="shared" si="13"/>
-        <v>-137951.4</v>
+        <v>-179951.4</v>
       </c>
       <c r="AZ61">
         <v>1</v>
@@ -17649,11 +17649,10 @@
       </c>
       <c r="AY62" s="1">
         <f t="shared" si="13"/>
-        <v>-157876.97719999999</v>
+        <v>-199876.97719999999</v>
       </c>
       <c r="AZ62">
-        <f t="shared" ref="AZ62:AZ63" si="21">7/12/100+1</f>
-        <v>1.0058333333333334</v>
+        <v>1</v>
       </c>
       <c r="BB62">
         <v>1.03</v>

</xml_diff>